<commit_message>
added confirm drawing & fixed choosing form
</commit_message>
<xml_diff>
--- a/public/examples/size.xlsx
+++ b/public/examples/size.xlsx
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
     <t xml:space="preserve">flange</t>
   </si>
   <si>
@@ -61,9 +64,6 @@
     <t xml:space="preserve">s3</t>
   </si>
   <si>
-    <t xml:space="preserve">adn</t>
-  </si>
-  <si>
     <t xml:space="preserve">1/2</t>
   </si>
   <si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">EN 1514-2</t>
   </si>
   <si>
-    <t xml:space="preserve">Adn = dn (мм)</t>
+    <t xml:space="preserve">count нужен для упорядочивания размеров</t>
   </si>
   <si>
     <t xml:space="preserve">ГОСТ 33259(12815) (трубопроводы)</t>
@@ -388,7 +388,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T26" activeCellId="0" sqref="T26"/>
+      <selection pane="topLeft" activeCell="T9" activeCellId="0" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -455,98 +455,98 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>47.8</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>31.8</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>19.1</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>14.2</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="N2" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>1500</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>901.7</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>679.5</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>616</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>577.9</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="N3" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>600</v>
       </c>
       <c r="Q3" s="3" t="n">
         <v>1</v>
@@ -563,43 +563,43 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="F4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>34.9</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>25.4</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>14.2</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="M4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="N4" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>15</v>
       </c>
       <c r="Q4" s="3" t="n">
         <v>2</v>
@@ -616,40 +616,40 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>34.9</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>25.4</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="L5" s="0" t="n">
         <v>4.5</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="M5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="N5" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>15</v>
       </c>
       <c r="Q5" s="3" t="n">
         <v>3</v>
@@ -666,33 +666,36 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>33259</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="C6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>2</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="G6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="L6" s="0" t="n">
         <v>2.3</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="N6" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="Q6" s="3" t="n">
@@ -706,39 +709,42 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>28759</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>773</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>749</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>724</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="L7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="M7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="N7" s="0" t="s">
         <v>31</v>
       </c>
       <c r="Q7" s="3" t="n">
@@ -757,7 +763,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="7"/>
       <c r="Q9" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="9"/>
       <c r="T9" s="10" t="s">

</xml_diff>